<commit_message>
The business layer is tested
</commit_message>
<xml_diff>
--- a/UniversityDatabaseWithAdo/MinMaxAvgExamIDGropId.xlsx
+++ b/UniversityDatabaseWithAdo/MinMaxAvgExamIDGropId.xlsx
@@ -172,13 +172,13 @@
         <v>2</v>
       </c>
       <c r="D5" s="0">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" s="0">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5" s="0">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6">
@@ -192,13 +192,13 @@
         <v>2</v>
       </c>
       <c r="D6" s="0">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E6" s="0">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F6" s="0">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Written documentation and tests
</commit_message>
<xml_diff>
--- a/UniversityDatabaseWithAdo/MinMaxAvgExamIDGropId.xlsx
+++ b/UniversityDatabaseWithAdo/MinMaxAvgExamIDGropId.xlsx
@@ -112,81 +112,81 @@
         <v>1</v>
       </c>
       <c r="D2" s="0">
-        <v>9.5</v>
+        <v>6.5</v>
       </c>
       <c r="E2" s="0">
         <v>10</v>
       </c>
       <c r="F2" s="0">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="0">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="0">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D3" s="0">
-        <v>8.5</v>
+        <v>5</v>
       </c>
       <c r="E3" s="0">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" s="0">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" s="0">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C4" s="0">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" s="0">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E4" s="0">
         <v>8</v>
       </c>
       <c r="F4" s="0">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" s="0">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C5" s="0">
         <v>2</v>
       </c>
       <c r="D5" s="0">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E5" s="0">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F5" s="0">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B6" s="0">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C6" s="0">
         <v>2</v>

</xml_diff>